<commit_message>
DF Set correct listener name and some other fixes.
</commit_message>
<xml_diff>
--- a/mes-plugins/mes-plugins-orders/src/main/resources/orders/public/resources/orderImportSchema_pl.xlsx
+++ b/mes-plugins/mes-plugins-orders/src/main/resources/orders/public/resources/orderImportSchema_pl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lupo/qcadoo-src/mes/mes-plugins/mes-plugins-orders/src/main/resources/orders/public/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7989261-78E7-1A41-874D-AD5845D42301}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BF7300-0E6C-244D-A95E-A687F0CC8297}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
             <family val="2"/>
             <charset val="238"/>
           </rPr>
-          <t>Określ numer produktu zdefiniowanego w qcadoo.</t>
+          <t>Podaj numer produktu zdefiniowanego w qcadoo.</t>
         </r>
       </text>
     </comment>
@@ -322,8 +322,7 @@
             <family val="2"/>
             <charset val="238"/>
           </rPr>
-          <t xml:space="preserve">Dana opcjonalna
-</t>
+          <t>Dana opcjonalna</t>
         </r>
       </text>
     </comment>
@@ -335,8 +334,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">qcadoo MES:
 </t>
@@ -345,8 +343,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
           </rPr>
           <t>Dana opcjonalna</t>
         </r>
@@ -360,8 +358,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">qcadoo MES:
 </t>
@@ -370,8 +367,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
           </rPr>
           <t>Dana opcjonalna</t>
         </r>
@@ -385,8 +382,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">qcadoo MES:
 </t>
@@ -395,8 +391,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">Dana opcjonalna. 
 </t>
@@ -405,8 +401,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
           </rPr>
           <t>Podaj numer zdefiniowanej w qcadoo technologii danego produktu. Jeśli nie wypełnisz kolumny zostanie uzupełniona technologia domyślna produktu.</t>
         </r>
@@ -420,8 +416,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">qcadoo MES:
 </t>
@@ -430,8 +425,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
           </rPr>
           <t xml:space="preserve">Dana opcjonalna. 
 </t>
@@ -440,8 +435,8 @@
           <rPr>
             <sz val="10"/>
             <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
+            <rFont val="Tahoma"/>
+            <family val="34"/>
           </rPr>
           <t>Podaj wartość zdefiniowaną w słowniku kategorii zleceń.</t>
         </r>
@@ -593,7 +588,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -625,10 +620,17 @@
       <charset val="238"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Tahoma"/>
+      <family val="34"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="34"/>
     </font>
   </fonts>
   <fills count="2">

</xml_diff>